<commit_message>
added: data test sql 30x
</commit_message>
<xml_diff>
--- a/experiment_sql.xlsx
+++ b/experiment_sql.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1505"/>
+  <dimension ref="A1:K1567"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -71194,6 +71194,2920 @@
         </is>
       </c>
     </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>2020-11-02 023205269015</t>
+        </is>
+      </c>
+      <c r="B1506" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>02:32:23.908355</t>
+        </is>
+      </c>
+      <c r="D1506" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1506" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1506" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1506" t="n">
+        <v>464000</v>
+      </c>
+      <c r="H1506" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I1506" s="5" t="n">
+        <v>44137.10561653953</v>
+      </c>
+      <c r="J1506" s="5" t="n">
+        <v>44137.10583227227</v>
+      </c>
+      <c r="K1506" t="inlineStr">
+        <is>
+          <t>0:00:18.639309</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>2020-11-02 023225793528</t>
+        </is>
+      </c>
+      <c r="B1507" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>02:32:25.793566</t>
+        </is>
+      </c>
+      <c r="D1507" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1507" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1507" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1507" t="n">
+        <v>464000</v>
+      </c>
+      <c r="H1507" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I1507" s="5" t="n">
+        <v>44137.10585409176</v>
+      </c>
+      <c r="J1507" s="5" t="n">
+        <v>44137.10585409183</v>
+      </c>
+      <c r="K1507" t="inlineStr">
+        <is>
+          <t>0:00:00.000006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>2020-11-02 030422139488</t>
+        </is>
+      </c>
+      <c r="B1508" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>03:04:40.944366</t>
+        </is>
+      </c>
+      <c r="D1508" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1508" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1508" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1508" t="n">
+        <v>464000</v>
+      </c>
+      <c r="H1508" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I1508" s="5" t="n">
+        <v>44137.12803402185</v>
+      </c>
+      <c r="J1508" s="5" t="n">
+        <v>44137.12825167052</v>
+      </c>
+      <c r="K1508" t="inlineStr">
+        <is>
+          <t>0:00:18.804845</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>2020-11-02 030442701269</t>
+        </is>
+      </c>
+      <c r="B1509" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>03:04:55.024872</t>
+        </is>
+      </c>
+      <c r="D1509" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1509" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1509" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1509" t="n">
+        <v>464000</v>
+      </c>
+      <c r="H1509" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I1509" s="5" t="n">
+        <v>44137.12827200543</v>
+      </c>
+      <c r="J1509" s="5" t="n">
+        <v>44137.12841463939</v>
+      </c>
+      <c r="K1509" t="inlineStr">
+        <is>
+          <t>0:00:12.323574</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>2020-11-02 030458738103</t>
+        </is>
+      </c>
+      <c r="B1510" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>03:05:36.391783</t>
+        </is>
+      </c>
+      <c r="D1510" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1510" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1510" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1510" t="n">
+        <v>928000</v>
+      </c>
+      <c r="H1510" t="n">
+        <v>4000</v>
+      </c>
+      <c r="I1510" s="5" t="n">
+        <v>44137.12845761693</v>
+      </c>
+      <c r="J1510" s="5" t="n">
+        <v>44137.12889342307</v>
+      </c>
+      <c r="K1510" t="inlineStr">
+        <is>
+          <t>0:00:37.653650</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>2020-11-02 030538066532</t>
+        </is>
+      </c>
+      <c r="B1511" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>03:06:02.816996</t>
+        </is>
+      </c>
+      <c r="D1511" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1511" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1511" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1511" t="n">
+        <v>928000</v>
+      </c>
+      <c r="H1511" t="n">
+        <v>4000</v>
+      </c>
+      <c r="I1511" s="5" t="n">
+        <v>44137.12891280709</v>
+      </c>
+      <c r="J1511" s="5" t="n">
+        <v>44137.12919927043</v>
+      </c>
+      <c r="K1511" t="inlineStr">
+        <is>
+          <t>0:00:24.750433</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>2020-11-02 030606546978</t>
+        </is>
+      </c>
+      <c r="B1512" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>03:07:03.765583</t>
+        </is>
+      </c>
+      <c r="D1512" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1512" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1512" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1512" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="H1512" t="n">
+        <v>6000</v>
+      </c>
+      <c r="I1512" s="5" t="n">
+        <v>44137.12924244187</v>
+      </c>
+      <c r="J1512" s="5" t="n">
+        <v>44137.12990469388</v>
+      </c>
+      <c r="K1512" t="inlineStr">
+        <is>
+          <t>0:00:57.218573</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>2020-11-02 030705404709</t>
+        </is>
+      </c>
+      <c r="B1513" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>03:07:42.804919</t>
+        </is>
+      </c>
+      <c r="D1513" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1513" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1513" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1513" t="n">
+        <v>1392000</v>
+      </c>
+      <c r="H1513" t="n">
+        <v>6000</v>
+      </c>
+      <c r="I1513" s="5" t="n">
+        <v>44137.12992366561</v>
+      </c>
+      <c r="J1513" s="5" t="n">
+        <v>44137.13035653803</v>
+      </c>
+      <c r="K1513" t="inlineStr">
+        <is>
+          <t>0:00:37.400177</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>2020-11-02 030746671026</t>
+        </is>
+      </c>
+      <c r="B1514" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>03:09:02.476345</t>
+        </is>
+      </c>
+      <c r="D1514" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1514" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1514" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1514" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="H1514" t="n">
+        <v>8000</v>
+      </c>
+      <c r="I1514" s="5" t="n">
+        <v>44137.13040128502</v>
+      </c>
+      <c r="J1514" s="5" t="n">
+        <v>44137.13127866105</v>
+      </c>
+      <c r="K1514" t="inlineStr">
+        <is>
+          <t>0:01:15.805289</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>2020-11-02 030904118391</t>
+        </is>
+      </c>
+      <c r="B1515" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>03:09:53.862520</t>
+        </is>
+      </c>
+      <c r="D1515" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1515" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1515" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1515" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="H1515" t="n">
+        <v>8000</v>
+      </c>
+      <c r="I1515" s="5" t="n">
+        <v>44137.13129766656</v>
+      </c>
+      <c r="J1515" s="5" t="n">
+        <v>44137.13187340847</v>
+      </c>
+      <c r="K1515" t="inlineStr">
+        <is>
+          <t>0:00:49.744101</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>2020-11-02 030957563394</t>
+        </is>
+      </c>
+      <c r="B1516" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>03:11:32.431265</t>
+        </is>
+      </c>
+      <c r="D1516" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1516" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1516" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1516" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="H1516" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I1516" s="5" t="n">
+        <v>44137.131916243</v>
+      </c>
+      <c r="J1516" s="5" t="n">
+        <v>44137.13301425026</v>
+      </c>
+      <c r="K1516" t="inlineStr">
+        <is>
+          <t>0:01:34.867828</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>2020-11-02 031134081442</t>
+        </is>
+      </c>
+      <c r="B1517" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>03:12:36.094471</t>
+        </is>
+      </c>
+      <c r="D1517" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1517" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1517" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1517" t="n">
+        <v>2320000</v>
+      </c>
+      <c r="H1517" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I1517" s="5" t="n">
+        <v>44137.13303335002</v>
+      </c>
+      <c r="J1517" s="5" t="n">
+        <v>44137.13375109294</v>
+      </c>
+      <c r="K1517" t="inlineStr">
+        <is>
+          <t>0:01:02.012988</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>2020-11-02 031239938762</t>
+        </is>
+      </c>
+      <c r="B1518" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>03:14:32.929478</t>
+        </is>
+      </c>
+      <c r="D1518" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1518" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1518" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1518" t="n">
+        <v>2784000</v>
+      </c>
+      <c r="H1518" t="n">
+        <v>12000</v>
+      </c>
+      <c r="I1518" s="5" t="n">
+        <v>44137.13379558752</v>
+      </c>
+      <c r="J1518" s="5" t="n">
+        <v>44137.13510335011</v>
+      </c>
+      <c r="K1518" t="inlineStr">
+        <is>
+          <t>0:01:52.990687</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>2020-11-02 031434580107</t>
+        </is>
+      </c>
+      <c r="B1519" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>03:15:48.930709</t>
+        </is>
+      </c>
+      <c r="D1519" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1519" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1519" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1519" t="n">
+        <v>2784000</v>
+      </c>
+      <c r="H1519" t="n">
+        <v>12000</v>
+      </c>
+      <c r="I1519" s="5" t="n">
+        <v>44137.13512245494</v>
+      </c>
+      <c r="J1519" s="5" t="n">
+        <v>44137.13598299399</v>
+      </c>
+      <c r="K1519" t="inlineStr">
+        <is>
+          <t>0:01:14.350574</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>2020-11-02 031552662952</t>
+        </is>
+      </c>
+      <c r="B1520" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>03:18:05.384089</t>
+        </is>
+      </c>
+      <c r="D1520" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1520" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1520" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1520" t="n">
+        <v>3248000</v>
+      </c>
+      <c r="H1520" t="n">
+        <v>14000</v>
+      </c>
+      <c r="I1520" s="5" t="n">
+        <v>44137.13602619158</v>
+      </c>
+      <c r="J1520" s="5" t="n">
+        <v>44137.13756231551</v>
+      </c>
+      <c r="K1520" t="inlineStr">
+        <is>
+          <t>0:02:12.721108</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>2020-11-02 031807027115</t>
+        </is>
+      </c>
+      <c r="B1521" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>03:19:34.304727</t>
+        </is>
+      </c>
+      <c r="D1521" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1521" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1521" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1521" t="n">
+        <v>3248000</v>
+      </c>
+      <c r="H1521" t="n">
+        <v>14000</v>
+      </c>
+      <c r="I1521" s="5" t="n">
+        <v>44137.13758133235</v>
+      </c>
+      <c r="J1521" s="5" t="n">
+        <v>44137.13859148887</v>
+      </c>
+      <c r="K1521" t="inlineStr">
+        <is>
+          <t>0:01:27.277524</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>2020-11-02 031938061041</t>
+        </is>
+      </c>
+      <c r="B1522" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>03:22:10.999230</t>
+        </is>
+      </c>
+      <c r="D1522" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1522" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1522" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1522" t="n">
+        <v>3712000</v>
+      </c>
+      <c r="H1522" t="n">
+        <v>16000</v>
+      </c>
+      <c r="I1522" s="5" t="n">
+        <v>44137.13863496576</v>
+      </c>
+      <c r="J1522" s="5" t="n">
+        <v>44137.14040508273</v>
+      </c>
+      <c r="K1522" t="inlineStr">
+        <is>
+          <t>0:02:32.938107</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>2020-11-02 032212657492</t>
+        </is>
+      </c>
+      <c r="B1523" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>03:23:52.361495</t>
+        </is>
+      </c>
+      <c r="D1523" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1523" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1523" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1523" t="n">
+        <v>3712000</v>
+      </c>
+      <c r="H1523" t="n">
+        <v>16000</v>
+      </c>
+      <c r="I1523" s="5" t="n">
+        <v>44137.14042427653</v>
+      </c>
+      <c r="J1523" s="5" t="n">
+        <v>44137.14157825704</v>
+      </c>
+      <c r="K1523" t="inlineStr">
+        <is>
+          <t>0:01:39.703915</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>2020-11-02 032356128174</t>
+        </is>
+      </c>
+      <c r="B1524" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>03:26:45.453297</t>
+        </is>
+      </c>
+      <c r="D1524" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1524" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1524" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1524" t="n">
+        <v>4176000</v>
+      </c>
+      <c r="H1524" t="n">
+        <v>18000</v>
+      </c>
+      <c r="I1524" s="5" t="n">
+        <v>44137.14162185388</v>
+      </c>
+      <c r="J1524" s="5" t="n">
+        <v>44137.14358163511</v>
+      </c>
+      <c r="K1524" t="inlineStr">
+        <is>
+          <t>0:02:49.325099</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>2020-11-02 032647120087</t>
+        </is>
+      </c>
+      <c r="B1525" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>03:28:39.697271</t>
+        </is>
+      </c>
+      <c r="D1525" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1525" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1525" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1525" t="n">
+        <v>4176000</v>
+      </c>
+      <c r="H1525" t="n">
+        <v>18000</v>
+      </c>
+      <c r="I1525" s="5" t="n">
+        <v>44137.14360092693</v>
+      </c>
+      <c r="J1525" s="5" t="n">
+        <v>44137.14490390272</v>
+      </c>
+      <c r="K1525" t="inlineStr">
+        <is>
+          <t>0:01:52.577108</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>2020-11-02 032843444874</t>
+        </is>
+      </c>
+      <c r="B1526" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>03:31:51.847028</t>
+        </is>
+      </c>
+      <c r="D1526" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1526" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1526" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1526" t="n">
+        <v>4640000</v>
+      </c>
+      <c r="H1526" t="n">
+        <v>20000</v>
+      </c>
+      <c r="I1526" s="5" t="n">
+        <v>44137.14494727863</v>
+      </c>
+      <c r="J1526" s="5" t="n">
+        <v>44137.14712785734</v>
+      </c>
+      <c r="K1526" t="inlineStr">
+        <is>
+          <t>0:03:08.402000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>2020-11-02 033153524266</t>
+        </is>
+      </c>
+      <c r="B1527" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>03:33:58.563973</t>
+        </is>
+      </c>
+      <c r="D1527" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1527" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1527" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1527" t="n">
+        <v>4640000</v>
+      </c>
+      <c r="H1527" t="n">
+        <v>20000</v>
+      </c>
+      <c r="I1527" s="5" t="n">
+        <v>44137.1471472716</v>
+      </c>
+      <c r="J1527" s="5" t="n">
+        <v>44137.14859449008</v>
+      </c>
+      <c r="K1527" t="inlineStr">
+        <is>
+          <t>0:02:05.039677</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>2020-11-02 033402385290</t>
+        </is>
+      </c>
+      <c r="B1528" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>03:37:30.078822</t>
+        </is>
+      </c>
+      <c r="D1528" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1528" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1528" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1528" t="n">
+        <v>5104000</v>
+      </c>
+      <c r="H1528" t="n">
+        <v>22000</v>
+      </c>
+      <c r="I1528" s="5" t="n">
+        <v>44137.14863871864</v>
+      </c>
+      <c r="J1528" s="5" t="n">
+        <v>44137.15104257863</v>
+      </c>
+      <c r="K1528" t="inlineStr">
+        <is>
+          <t>0:03:27.693504</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>2020-11-02 033731770679</t>
+        </is>
+      </c>
+      <c r="B1529" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>03:39:49.791546</t>
+        </is>
+      </c>
+      <c r="D1529" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1529" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1529" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1529" t="n">
+        <v>5104000</v>
+      </c>
+      <c r="H1529" t="n">
+        <v>22000</v>
+      </c>
+      <c r="I1529" s="5" t="n">
+        <v>44137.15106216065</v>
+      </c>
+      <c r="J1529" s="5" t="n">
+        <v>44137.15265962409</v>
+      </c>
+      <c r="K1529" t="inlineStr">
+        <is>
+          <t>0:02:18.020842</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>2020-11-02 033953535670</t>
+        </is>
+      </c>
+      <c r="B1530" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>03:43:39.418048</t>
+        </is>
+      </c>
+      <c r="D1530" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1530" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1530" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1530" t="n">
+        <v>5568000</v>
+      </c>
+      <c r="H1530" t="n">
+        <v>24000</v>
+      </c>
+      <c r="I1530" s="5" t="n">
+        <v>44137.15270295915</v>
+      </c>
+      <c r="J1530" s="5" t="n">
+        <v>44137.15531733816</v>
+      </c>
+      <c r="K1530" t="inlineStr">
+        <is>
+          <t>0:03:45.882347</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr">
+        <is>
+          <t>2020-11-02 034341066619</t>
+        </is>
+      </c>
+      <c r="B1531" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>03:46:11.328394</t>
+        </is>
+      </c>
+      <c r="D1531" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1531" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1531" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1531" t="n">
+        <v>5568000</v>
+      </c>
+      <c r="H1531" t="n">
+        <v>24000</v>
+      </c>
+      <c r="I1531" s="5" t="n">
+        <v>44137.1553364192</v>
+      </c>
+      <c r="J1531" s="5" t="n">
+        <v>44137.15707555925</v>
+      </c>
+      <c r="K1531" t="inlineStr">
+        <is>
+          <t>0:02:30.261700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>2020-11-02 034615141174</t>
+        </is>
+      </c>
+      <c r="B1532" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>03:50:21.206630</t>
+        </is>
+      </c>
+      <c r="D1532" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1532" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1532" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1532" t="n">
+        <v>6032000</v>
+      </c>
+      <c r="H1532" t="n">
+        <v>26000</v>
+      </c>
+      <c r="I1532" s="5" t="n">
+        <v>44137.15711968952</v>
+      </c>
+      <c r="J1532" s="5" t="n">
+        <v>44137.15996766897</v>
+      </c>
+      <c r="K1532" t="inlineStr">
+        <is>
+          <t>0:04:06.065425</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="inlineStr">
+        <is>
+          <t>2020-11-02 035022856405</t>
+        </is>
+      </c>
+      <c r="B1533" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>03:53:05.602304</t>
+        </is>
+      </c>
+      <c r="D1533" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1533" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1533" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1533" t="n">
+        <v>6032000</v>
+      </c>
+      <c r="H1533" t="n">
+        <v>26000</v>
+      </c>
+      <c r="I1533" s="5" t="n">
+        <v>44137.15998676395</v>
+      </c>
+      <c r="J1533" s="5" t="n">
+        <v>44137.161870396</v>
+      </c>
+      <c r="K1533" t="inlineStr">
+        <is>
+          <t>0:02:42.745809</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr">
+        <is>
+          <t>2020-11-02 035309427298</t>
+        </is>
+      </c>
+      <c r="B1534" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>03:57:33.354833</t>
+        </is>
+      </c>
+      <c r="D1534" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1534" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1534" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1534" t="n">
+        <v>6496000</v>
+      </c>
+      <c r="H1534" t="n">
+        <v>28000</v>
+      </c>
+      <c r="I1534" s="5" t="n">
+        <v>44137.1619146678</v>
+      </c>
+      <c r="J1534" s="5" t="n">
+        <v>44137.16496938431</v>
+      </c>
+      <c r="K1534" t="inlineStr">
+        <is>
+          <t>0:04:23.927506</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr">
+        <is>
+          <t>2020-11-02 035735034982</t>
+        </is>
+      </c>
+      <c r="B1535" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>04:00:30.691027</t>
+        </is>
+      </c>
+      <c r="D1535" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1535" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1535" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1535" t="n">
+        <v>6496000</v>
+      </c>
+      <c r="H1535" t="n">
+        <v>28000</v>
+      </c>
+      <c r="I1535" s="5" t="n">
+        <v>44137.16498883081</v>
+      </c>
+      <c r="J1535" s="5" t="n">
+        <v>44137.16702188654</v>
+      </c>
+      <c r="K1535" t="inlineStr">
+        <is>
+          <t>0:02:55.656015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr">
+        <is>
+          <t>2020-11-02 040034485873</t>
+        </is>
+      </c>
+      <c r="B1536" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>04:05:17.139568</t>
+        </is>
+      </c>
+      <c r="D1536" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1536" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1536" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1536" t="n">
+        <v>6960000</v>
+      </c>
+      <c r="H1536" t="n">
+        <v>30000</v>
+      </c>
+      <c r="I1536" s="5" t="n">
+        <v>44137.16706580872</v>
+      </c>
+      <c r="J1536" s="5" t="n">
+        <v>44137.1703372632</v>
+      </c>
+      <c r="K1536" t="inlineStr">
+        <is>
+          <t>0:04:42.653668</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="inlineStr">
+        <is>
+          <t>2020-11-02 040518812056</t>
+        </is>
+      </c>
+      <c r="B1537" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>04:08:26.872120</t>
+        </is>
+      </c>
+      <c r="D1537" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1537" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1537" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1537" t="n">
+        <v>6960000</v>
+      </c>
+      <c r="H1537" t="n">
+        <v>30000</v>
+      </c>
+      <c r="I1537" s="5" t="n">
+        <v>44137.17035662102</v>
+      </c>
+      <c r="J1537" s="5" t="n">
+        <v>44137.17253324181</v>
+      </c>
+      <c r="K1537" t="inlineStr">
+        <is>
+          <t>0:03:08.060036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr">
+        <is>
+          <t>2020-11-02 040830674295</t>
+        </is>
+      </c>
+      <c r="B1538" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>04:13:32.608160</t>
+        </is>
+      </c>
+      <c r="D1538" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1538" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1538" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1538" t="n">
+        <v>7424000</v>
+      </c>
+      <c r="H1538" t="n">
+        <v>32000</v>
+      </c>
+      <c r="I1538" s="5" t="n">
+        <v>44137.17257724877</v>
+      </c>
+      <c r="J1538" s="5" t="n">
+        <v>44137.17607185343</v>
+      </c>
+      <c r="K1538" t="inlineStr">
+        <is>
+          <t>0:05:01.933841</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" t="inlineStr">
+        <is>
+          <t>2020-11-02 041334280036</t>
+        </is>
+      </c>
+      <c r="B1539" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>04:16:54.895430</t>
+        </is>
+      </c>
+      <c r="D1539" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1539" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1539" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1539" t="n">
+        <v>7424000</v>
+      </c>
+      <c r="H1539" t="n">
+        <v>32000</v>
+      </c>
+      <c r="I1539" s="5" t="n">
+        <v>44137.17609120412</v>
+      </c>
+      <c r="J1539" s="5" t="n">
+        <v>44137.17841314121</v>
+      </c>
+      <c r="K1539" t="inlineStr">
+        <is>
+          <t>0:03:20.615364</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" t="inlineStr">
+        <is>
+          <t>2020-11-02 041658817539</t>
+        </is>
+      </c>
+      <c r="B1540" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>04:22:19.943736</t>
+        </is>
+      </c>
+      <c r="D1540" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1540" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1540" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1540" t="n">
+        <v>7888000</v>
+      </c>
+      <c r="H1540" t="n">
+        <v>34000</v>
+      </c>
+      <c r="I1540" s="5" t="n">
+        <v>44137.17845853633</v>
+      </c>
+      <c r="J1540" s="5" t="n">
+        <v>44137.18217527438</v>
+      </c>
+      <c r="K1540" t="inlineStr">
+        <is>
+          <t>0:05:21.126167</t>
+        </is>
+      </c>
+    </row>
+    <row r="1541">
+      <c r="A1541" t="inlineStr">
+        <is>
+          <t>2020-11-02 042221617041</t>
+        </is>
+      </c>
+      <c r="B1541" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1541" t="inlineStr">
+        <is>
+          <t>04:25:54.520668</t>
+        </is>
+      </c>
+      <c r="D1541" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1541" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1541" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1541" t="n">
+        <v>7888000</v>
+      </c>
+      <c r="H1541" t="n">
+        <v>34000</v>
+      </c>
+      <c r="I1541" s="5" t="n">
+        <v>44137.18219464167</v>
+      </c>
+      <c r="J1541" s="5" t="n">
+        <v>44137.18465880369</v>
+      </c>
+      <c r="K1541" t="inlineStr">
+        <is>
+          <t>0:03:32.903598</t>
+        </is>
+      </c>
+    </row>
+    <row r="1542">
+      <c r="A1542" t="inlineStr">
+        <is>
+          <t>2020-11-02 042558374174</t>
+        </is>
+      </c>
+      <c r="B1542" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1542" t="inlineStr">
+        <is>
+          <t>04:31:39.114184</t>
+        </is>
+      </c>
+      <c r="D1542" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1542" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1542" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1542" t="n">
+        <v>8352000</v>
+      </c>
+      <c r="H1542" t="n">
+        <v>36000</v>
+      </c>
+      <c r="I1542" s="5" t="n">
+        <v>44137.18470340479</v>
+      </c>
+      <c r="J1542" s="5" t="n">
+        <v>44137.18864715462</v>
+      </c>
+      <c r="K1542" t="inlineStr">
+        <is>
+          <t>0:05:40.739985</t>
+        </is>
+      </c>
+    </row>
+    <row r="1543">
+      <c r="A1543" t="inlineStr">
+        <is>
+          <t>2020-11-02 043140753740</t>
+        </is>
+      </c>
+      <c r="B1543" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1543" t="inlineStr">
+        <is>
+          <t>04:35:26.120643</t>
+        </is>
+      </c>
+      <c r="D1543" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1543" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1543" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1543" t="n">
+        <v>8352000</v>
+      </c>
+      <c r="H1543" t="n">
+        <v>36000</v>
+      </c>
+      <c r="I1543" s="5" t="n">
+        <v>44137.18866613125</v>
+      </c>
+      <c r="J1543" s="5" t="n">
+        <v>44137.19127454419</v>
+      </c>
+      <c r="K1543" t="inlineStr">
+        <is>
+          <t>0:03:45.366878</t>
+        </is>
+      </c>
+    </row>
+    <row r="1544">
+      <c r="A1544" t="inlineStr">
+        <is>
+          <t>2020-11-02 043529912988</t>
+        </is>
+      </c>
+      <c r="B1544" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1544" t="inlineStr">
+        <is>
+          <t>04:41:28.880396</t>
+        </is>
+      </c>
+      <c r="D1544" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1544" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1544" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1544" t="n">
+        <v>8816000</v>
+      </c>
+      <c r="H1544" t="n">
+        <v>38000</v>
+      </c>
+      <c r="I1544" s="5" t="n">
+        <v>44137.19131843736</v>
+      </c>
+      <c r="J1544" s="5" t="n">
+        <v>44137.19547315242</v>
+      </c>
+      <c r="K1544" t="inlineStr">
+        <is>
+          <t>0:05:58.967381</t>
+        </is>
+      </c>
+    </row>
+    <row r="1545">
+      <c r="A1545" t="inlineStr">
+        <is>
+          <t>2020-11-02 044130537967</t>
+        </is>
+      </c>
+      <c r="B1545" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1545" t="inlineStr">
+        <is>
+          <t>04:45:28.628921</t>
+        </is>
+      </c>
+      <c r="D1545" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1545" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1545" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1545" t="n">
+        <v>8816000</v>
+      </c>
+      <c r="H1545" t="n">
+        <v>38000</v>
+      </c>
+      <c r="I1545" s="5" t="n">
+        <v>44137.19549233758</v>
+      </c>
+      <c r="J1545" s="5" t="n">
+        <v>44137.19824801962</v>
+      </c>
+      <c r="K1545" t="inlineStr">
+        <is>
+          <t>0:03:58.090928</t>
+        </is>
+      </c>
+    </row>
+    <row r="1546">
+      <c r="A1546" t="inlineStr">
+        <is>
+          <t>2020-11-02 044532465360</t>
+        </is>
+      </c>
+      <c r="B1546" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1546" t="inlineStr">
+        <is>
+          <t>04:51:49.856181</t>
+        </is>
+      </c>
+      <c r="D1546" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1546" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1546" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1546" t="n">
+        <v>9280000</v>
+      </c>
+      <c r="H1546" t="n">
+        <v>40000</v>
+      </c>
+      <c r="I1546" s="5" t="n">
+        <v>44137.19829242315</v>
+      </c>
+      <c r="J1546" s="5" t="n">
+        <v>44137.20266037212</v>
+      </c>
+      <c r="K1546" t="inlineStr">
+        <is>
+          <t>0:06:17.390791</t>
+        </is>
+      </c>
+    </row>
+    <row r="1547">
+      <c r="A1547" t="inlineStr">
+        <is>
+          <t>2020-11-02 045151488914</t>
+        </is>
+      </c>
+      <c r="B1547" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1547" t="inlineStr">
+        <is>
+          <t>04:56:01.939391</t>
+        </is>
+      </c>
+      <c r="D1547" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1547" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1547" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1547" t="n">
+        <v>9280000</v>
+      </c>
+      <c r="H1547" t="n">
+        <v>40000</v>
+      </c>
+      <c r="I1547" s="5" t="n">
+        <v>44137.20267926984</v>
+      </c>
+      <c r="J1547" s="5" t="n">
+        <v>44137.20557800191</v>
+      </c>
+      <c r="K1547" t="inlineStr">
+        <is>
+          <t>0:04:10.450451</t>
+        </is>
+      </c>
+    </row>
+    <row r="1548">
+      <c r="A1548" t="inlineStr">
+        <is>
+          <t>2020-11-02 045605764943</t>
+        </is>
+      </c>
+      <c r="B1548" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1548" t="inlineStr">
+        <is>
+          <t>05:02:42.885815</t>
+        </is>
+      </c>
+      <c r="D1548" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1548" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1548" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1548" t="n">
+        <v>9744000</v>
+      </c>
+      <c r="H1548" t="n">
+        <v>42000</v>
+      </c>
+      <c r="I1548" s="5" t="n">
+        <v>44137.20562227943</v>
+      </c>
+      <c r="J1548" s="5" t="n">
+        <v>44137.21021858546</v>
+      </c>
+      <c r="K1548" t="inlineStr">
+        <is>
+          <t>0:06:37.120842</t>
+        </is>
+      </c>
+    </row>
+    <row r="1549">
+      <c r="A1549" t="inlineStr">
+        <is>
+          <t>2020-11-02 050244569903</t>
+        </is>
+      </c>
+      <c r="B1549" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1549" t="inlineStr">
+        <is>
+          <t>05:07:07.736523</t>
+        </is>
+      </c>
+      <c r="D1549" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1549" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1549" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1549" t="n">
+        <v>9744000</v>
+      </c>
+      <c r="H1549" t="n">
+        <v>42000</v>
+      </c>
+      <c r="I1549" s="5" t="n">
+        <v>44137.21023807758</v>
+      </c>
+      <c r="J1549" s="5" t="n">
+        <v>44137.21328398724</v>
+      </c>
+      <c r="K1549" t="inlineStr">
+        <is>
+          <t>0:04:23.166594</t>
+        </is>
+      </c>
+    </row>
+    <row r="1550">
+      <c r="A1550" t="inlineStr">
+        <is>
+          <t>2020-11-02 050711542719</t>
+        </is>
+      </c>
+      <c r="B1550" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1550" t="inlineStr">
+        <is>
+          <t>05:14:07.723003</t>
+        </is>
+      </c>
+      <c r="D1550" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1550" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1550" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1550" t="n">
+        <v>10208000</v>
+      </c>
+      <c r="H1550" t="n">
+        <v>44000</v>
+      </c>
+      <c r="I1550" s="5" t="n">
+        <v>44137.21332804073</v>
+      </c>
+      <c r="J1550" s="5" t="n">
+        <v>44137.21814494183</v>
+      </c>
+      <c r="K1550" t="inlineStr">
+        <is>
+          <t>0:06:56.180255</t>
+        </is>
+      </c>
+    </row>
+    <row r="1551">
+      <c r="A1551" t="inlineStr">
+        <is>
+          <t>2020-11-02 051409400022</t>
+        </is>
+      </c>
+      <c r="B1551" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1551" t="inlineStr">
+        <is>
+          <t>05:18:44.519661</t>
+        </is>
+      </c>
+      <c r="D1551" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1551" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1551" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1551" t="n">
+        <v>10208000</v>
+      </c>
+      <c r="H1551" t="n">
+        <v>44000</v>
+      </c>
+      <c r="I1551" s="5" t="n">
+        <v>44137.2181643521</v>
+      </c>
+      <c r="J1551" s="5" t="n">
+        <v>44137.22134860689</v>
+      </c>
+      <c r="K1551" t="inlineStr">
+        <is>
+          <t>0:04:35.119613</t>
+        </is>
+      </c>
+    </row>
+    <row r="1552">
+      <c r="A1552" t="inlineStr">
+        <is>
+          <t>2020-11-02 051848362531</t>
+        </is>
+      </c>
+      <c r="B1552" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1552" t="inlineStr">
+        <is>
+          <t>05:26:02.483857</t>
+        </is>
+      </c>
+      <c r="D1552" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1552" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1552" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1552" t="n">
+        <v>10672000</v>
+      </c>
+      <c r="H1552" t="n">
+        <v>46000</v>
+      </c>
+      <c r="I1552" s="5" t="n">
+        <v>44137.22139308485</v>
+      </c>
+      <c r="J1552" s="5" t="n">
+        <v>44137.22641763688</v>
+      </c>
+      <c r="K1552" t="inlineStr">
+        <is>
+          <t>0:07:14.121296</t>
+        </is>
+      </c>
+    </row>
+    <row r="1553">
+      <c r="A1553" t="inlineStr">
+        <is>
+          <t>2020-11-02 052604151956</t>
+        </is>
+      </c>
+      <c r="B1553" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1553" t="inlineStr">
+        <is>
+          <t>05:30:51.817197</t>
+        </is>
+      </c>
+      <c r="D1553" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1553" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1553" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1553" t="n">
+        <v>10672000</v>
+      </c>
+      <c r="H1553" t="n">
+        <v>46000</v>
+      </c>
+      <c r="I1553" s="5" t="n">
+        <v>44137.22643694394</v>
+      </c>
+      <c r="J1553" s="5" t="n">
+        <v>44137.2297664018</v>
+      </c>
+      <c r="K1553" t="inlineStr">
+        <is>
+          <t>0:04:47.665159</t>
+        </is>
+      </c>
+    </row>
+    <row r="1554">
+      <c r="A1554" t="inlineStr">
+        <is>
+          <t>2020-11-02 053055617898</t>
+        </is>
+      </c>
+      <c r="B1554" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1554" t="inlineStr">
+        <is>
+          <t>05:38:30.457024</t>
+        </is>
+      </c>
+      <c r="D1554" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1554" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1554" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1554" t="n">
+        <v>11136000</v>
+      </c>
+      <c r="H1554" t="n">
+        <v>48000</v>
+      </c>
+      <c r="I1554" s="5" t="n">
+        <v>44137.22981039234</v>
+      </c>
+      <c r="J1554" s="5" t="n">
+        <v>44137.23507473374</v>
+      </c>
+      <c r="K1554" t="inlineStr">
+        <is>
+          <t>0:07:34.839096</t>
+        </is>
+      </c>
+    </row>
+    <row r="1555">
+      <c r="A1555" t="inlineStr">
+        <is>
+          <t>2020-11-02 053832155977</t>
+        </is>
+      </c>
+      <c r="B1555" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1555" t="inlineStr">
+        <is>
+          <t>05:43:32.693551</t>
+        </is>
+      </c>
+      <c r="D1555" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1555" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1555" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1555" t="n">
+        <v>11136000</v>
+      </c>
+      <c r="H1555" t="n">
+        <v>48000</v>
+      </c>
+      <c r="I1555" s="5" t="n">
+        <v>44137.23509439788</v>
+      </c>
+      <c r="J1555" s="5" t="n">
+        <v>44137.2385728417</v>
+      </c>
+      <c r="K1555" t="inlineStr">
+        <is>
+          <t>0:05:00.537547</t>
+        </is>
+      </c>
+    </row>
+    <row r="1556">
+      <c r="A1556" t="inlineStr">
+        <is>
+          <t>2020-11-02 054336531379</t>
+        </is>
+      </c>
+      <c r="B1556" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1556" t="inlineStr">
+        <is>
+          <t>05:51:28.356099</t>
+        </is>
+      </c>
+      <c r="D1556" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1556" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1556" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1556" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="H1556" t="n">
+        <v>50000</v>
+      </c>
+      <c r="I1556" s="5" t="n">
+        <v>44137.23861726133</v>
+      </c>
+      <c r="J1556" s="5" t="n">
+        <v>44137.24407819525</v>
+      </c>
+      <c r="K1556" t="inlineStr">
+        <is>
+          <t>0:07:51.824690</t>
+        </is>
+      </c>
+    </row>
+    <row r="1557">
+      <c r="A1557" t="inlineStr">
+        <is>
+          <t>2020-11-02 055130018482</t>
+        </is>
+      </c>
+      <c r="B1557" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1557" t="inlineStr">
+        <is>
+          <t>05:56:42.942216</t>
+        </is>
+      </c>
+      <c r="D1557" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1557" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1557" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1557" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="H1557" t="n">
+        <v>50000</v>
+      </c>
+      <c r="I1557" s="5" t="n">
+        <v>44137.24409743613</v>
+      </c>
+      <c r="J1557" s="5" t="n">
+        <v>44137.2477192383</v>
+      </c>
+      <c r="K1557" t="inlineStr">
+        <is>
+          <t>0:05:12.923707</t>
+        </is>
+      </c>
+    </row>
+    <row r="1558">
+      <c r="A1558" t="inlineStr">
+        <is>
+          <t>2020-11-02 055646862928</t>
+        </is>
+      </c>
+      <c r="B1558" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1558" t="inlineStr">
+        <is>
+          <t>06:04:58.752134</t>
+        </is>
+      </c>
+      <c r="D1558" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1558" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1558" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1558" t="n">
+        <v>12064000</v>
+      </c>
+      <c r="H1558" t="n">
+        <v>52000</v>
+      </c>
+      <c r="I1558" s="5" t="n">
+        <v>44137.24776461722</v>
+      </c>
+      <c r="J1558" s="5" t="n">
+        <v>44137.25345777903</v>
+      </c>
+      <c r="K1558" t="inlineStr">
+        <is>
+          <t>0:08:11.889180</t>
+        </is>
+      </c>
+    </row>
+    <row r="1559">
+      <c r="A1559" t="inlineStr">
+        <is>
+          <t>2020-11-02 060500430204</t>
+        </is>
+      </c>
+      <c r="B1559" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1559" t="inlineStr">
+        <is>
+          <t>06:10:25.971733</t>
+        </is>
+      </c>
+      <c r="D1559" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1559" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1559" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1559" t="n">
+        <v>12064000</v>
+      </c>
+      <c r="H1559" t="n">
+        <v>52000</v>
+      </c>
+      <c r="I1559" s="5" t="n">
+        <v>44137.25347720143</v>
+      </c>
+      <c r="J1559" s="5" t="n">
+        <v>44137.25724504286</v>
+      </c>
+      <c r="K1559" t="inlineStr">
+        <is>
+          <t>0:05:25.541499</t>
+        </is>
+      </c>
+    </row>
+    <row r="1560">
+      <c r="A1560" t="inlineStr">
+        <is>
+          <t>2020-11-02 061029892190</t>
+        </is>
+      </c>
+      <c r="B1560" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1560" t="inlineStr">
+        <is>
+          <t>06:19:07.230994</t>
+        </is>
+      </c>
+      <c r="D1560" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1560" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1560" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1560" t="n">
+        <v>12528000</v>
+      </c>
+      <c r="H1560" t="n">
+        <v>54000</v>
+      </c>
+      <c r="I1560" s="5" t="n">
+        <v>44137.25729041886</v>
+      </c>
+      <c r="J1560" s="5" t="n">
+        <v>44137.26327813616</v>
+      </c>
+      <c r="K1560" t="inlineStr">
+        <is>
+          <t>0:08:37.338774</t>
+        </is>
+      </c>
+    </row>
+    <row r="1561">
+      <c r="A1561" t="inlineStr">
+        <is>
+          <t>2020-11-02 061908955565</t>
+        </is>
+      </c>
+      <c r="B1561" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1561" t="inlineStr">
+        <is>
+          <t>06:24:49.269301</t>
+        </is>
+      </c>
+      <c r="D1561" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1561" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1561" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1561" t="n">
+        <v>12528000</v>
+      </c>
+      <c r="H1561" t="n">
+        <v>54000</v>
+      </c>
+      <c r="I1561" s="5" t="n">
+        <v>44137.26329809682</v>
+      </c>
+      <c r="J1561" s="5" t="n">
+        <v>44137.26723691286</v>
+      </c>
+      <c r="K1561" t="inlineStr">
+        <is>
+          <t>0:05:40.313706</t>
+        </is>
+      </c>
+    </row>
+    <row r="1562">
+      <c r="A1562" t="inlineStr">
+        <is>
+          <t>2020-11-02 062453169408</t>
+        </is>
+      </c>
+      <c r="B1562" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1562" t="inlineStr">
+        <is>
+          <t>06:33:47.562763</t>
+        </is>
+      </c>
+      <c r="D1562" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1562" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1562" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1562" t="n">
+        <v>12992000</v>
+      </c>
+      <c r="H1562" t="n">
+        <v>56000</v>
+      </c>
+      <c r="I1562" s="5" t="n">
+        <v>44137.26728205333</v>
+      </c>
+      <c r="J1562" s="5" t="n">
+        <v>44137.27346716132</v>
+      </c>
+      <c r="K1562" t="inlineStr">
+        <is>
+          <t>0:08:54.393330</t>
+        </is>
+      </c>
+    </row>
+    <row r="1563">
+      <c r="A1563" t="inlineStr">
+        <is>
+          <t>2020-11-02 063349226822</t>
+        </is>
+      </c>
+      <c r="B1563" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1563" t="inlineStr">
+        <is>
+          <t>06:39:39.770852</t>
+        </is>
+      </c>
+      <c r="D1563" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1563" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1563" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1563" t="n">
+        <v>12992000</v>
+      </c>
+      <c r="H1563" t="n">
+        <v>56000</v>
+      </c>
+      <c r="I1563" s="5" t="n">
+        <v>44137.27348642155</v>
+      </c>
+      <c r="J1563" s="5" t="n">
+        <v>44137.27754364381</v>
+      </c>
+      <c r="K1563" t="inlineStr">
+        <is>
+          <t>0:05:50.544002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1564">
+      <c r="A1564" t="inlineStr">
+        <is>
+          <t>2020-11-02 063943642477</t>
+        </is>
+      </c>
+      <c r="B1564" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1564" t="inlineStr">
+        <is>
+          <t>06:48:51.755872</t>
+        </is>
+      </c>
+      <c r="D1564" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1564" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1564" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1564" t="n">
+        <v>13456000</v>
+      </c>
+      <c r="H1564" t="n">
+        <v>58000</v>
+      </c>
+      <c r="I1564" s="5" t="n">
+        <v>44137.27758845459</v>
+      </c>
+      <c r="J1564" s="5" t="n">
+        <v>44137.28393235931</v>
+      </c>
+      <c r="K1564" t="inlineStr">
+        <is>
+          <t>0:09:08.113368</t>
+        </is>
+      </c>
+    </row>
+    <row r="1565">
+      <c r="A1565" t="inlineStr">
+        <is>
+          <t>2020-11-02 064853426513</t>
+        </is>
+      </c>
+      <c r="B1565" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1565" t="inlineStr">
+        <is>
+          <t>06:54:56.780674</t>
+        </is>
+      </c>
+      <c r="D1565" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1565" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1565" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1565" t="n">
+        <v>13456000</v>
+      </c>
+      <c r="H1565" t="n">
+        <v>58000</v>
+      </c>
+      <c r="I1565" s="5" t="n">
+        <v>44137.28395169574</v>
+      </c>
+      <c r="J1565" s="5" t="n">
+        <v>44137.28815718342</v>
+      </c>
+      <c r="K1565" t="inlineStr">
+        <is>
+          <t>0:06:03.354135</t>
+        </is>
+      </c>
+    </row>
+    <row r="1566">
+      <c r="A1566" t="inlineStr">
+        <is>
+          <t>2020-11-02 065500672251</t>
+        </is>
+      </c>
+      <c r="B1566" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1566" t="inlineStr">
+        <is>
+          <t>07:04:26.861509</t>
+        </is>
+      </c>
+      <c r="D1566" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1566" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1566" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1566" t="n">
+        <v>13920000</v>
+      </c>
+      <c r="H1566" t="n">
+        <v>60000</v>
+      </c>
+      <c r="I1566" s="5" t="n">
+        <v>44137.28820222513</v>
+      </c>
+      <c r="J1566" s="5" t="n">
+        <v>44137.29475534119</v>
+      </c>
+      <c r="K1566" t="inlineStr">
+        <is>
+          <t>0:09:26.189228</t>
+        </is>
+      </c>
+    </row>
+    <row r="1567">
+      <c r="A1567" t="inlineStr">
+        <is>
+          <t>2020-11-02 070428505580</t>
+        </is>
+      </c>
+      <c r="B1567" s="4" t="n">
+        <v>44137</v>
+      </c>
+      <c r="C1567" t="inlineStr">
+        <is>
+          <t>07:10:44.403371</t>
+        </is>
+      </c>
+      <c r="D1567" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1567" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1567" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1567" t="n">
+        <v>13920000</v>
+      </c>
+      <c r="H1567" t="n">
+        <v>60000</v>
+      </c>
+      <c r="I1567" s="5" t="n">
+        <v>44137.29477437014</v>
+      </c>
+      <c r="J1567" s="5" t="n">
+        <v>44137.29912503868</v>
+      </c>
+      <c r="K1567" t="inlineStr">
+        <is>
+          <t>0:06:15.897762</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
added 50000x tests sql
</commit_message>
<xml_diff>
--- a/experiment_sql.xlsx
+++ b/experiment_sql.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1567"/>
+  <dimension ref="A1:K1607"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -74108,6 +74108,1886 @@
         </is>
       </c>
     </row>
+    <row r="1568">
+      <c r="A1568" t="inlineStr">
+        <is>
+          <t>2020-11-23 015355930651</t>
+        </is>
+      </c>
+      <c r="B1568" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1568" t="inlineStr">
+        <is>
+          <t>02:01:54.419743</t>
+        </is>
+      </c>
+      <c r="D1568" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1568" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1568" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1568" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="H1568" t="n">
+        <v>50000</v>
+      </c>
+      <c r="I1568" s="5" t="n">
+        <v>44158.07911956772</v>
+      </c>
+      <c r="J1568" s="5" t="n">
+        <v>44158.08465763555</v>
+      </c>
+      <c r="K1568" t="inlineStr">
+        <is>
+          <t>0:07:58.489061</t>
+        </is>
+      </c>
+    </row>
+    <row r="1569">
+      <c r="A1569" t="inlineStr">
+        <is>
+          <t>2020-11-23 020156422300</t>
+        </is>
+      </c>
+      <c r="B1569" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1569" t="inlineStr">
+        <is>
+          <t>02:07:06.753747</t>
+        </is>
+      </c>
+      <c r="D1569" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1569" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1569" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1569" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="H1569" t="n">
+        <v>50000</v>
+      </c>
+      <c r="I1569" s="5" t="n">
+        <v>44158.08468081366</v>
+      </c>
+      <c r="J1569" s="5" t="n">
+        <v>44158.08827261244</v>
+      </c>
+      <c r="K1569" t="inlineStr">
+        <is>
+          <t>0:05:10.331416</t>
+        </is>
+      </c>
+    </row>
+    <row r="1570">
+      <c r="A1570" t="inlineStr">
+        <is>
+          <t>2020-11-23 020710683597</t>
+        </is>
+      </c>
+      <c r="B1570" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1570" t="inlineStr">
+        <is>
+          <t>02:23:08.862832</t>
+        </is>
+      </c>
+      <c r="D1570" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1570" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1570" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1570" t="n">
+        <v>23200000</v>
+      </c>
+      <c r="H1570" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I1570" s="5" t="n">
+        <v>44158.08831809719</v>
+      </c>
+      <c r="J1570" s="5" t="n">
+        <v>44158.09940813428</v>
+      </c>
+      <c r="K1570" t="inlineStr">
+        <is>
+          <t>0:15:58.179206</t>
+        </is>
+      </c>
+    </row>
+    <row r="1571">
+      <c r="A1571" t="inlineStr">
+        <is>
+          <t>2020-11-23 022310564345</t>
+        </is>
+      </c>
+      <c r="B1571" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1571" t="inlineStr">
+        <is>
+          <t>02:33:31.923094</t>
+        </is>
+      </c>
+      <c r="D1571" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1571" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1571" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1571" t="n">
+        <v>23200000</v>
+      </c>
+      <c r="H1571" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I1571" s="5" t="n">
+        <v>44158.09942782807</v>
+      </c>
+      <c r="J1571" s="5" t="n">
+        <v>44158.10661947994</v>
+      </c>
+      <c r="K1571" t="inlineStr">
+        <is>
+          <t>0:10:21.358722</t>
+        </is>
+      </c>
+    </row>
+    <row r="1572">
+      <c r="A1572" t="inlineStr">
+        <is>
+          <t>2020-11-23 023335956474</t>
+        </is>
+      </c>
+      <c r="B1572" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1572" t="inlineStr">
+        <is>
+          <t>02:57:23.764309</t>
+        </is>
+      </c>
+      <c r="D1572" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1572" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1572" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1572" t="n">
+        <v>34800000</v>
+      </c>
+      <c r="H1572" t="n">
+        <v>150000</v>
+      </c>
+      <c r="I1572" s="5" t="n">
+        <v>44158.10666616288</v>
+      </c>
+      <c r="J1572" s="5" t="n">
+        <v>44158.12319171623</v>
+      </c>
+      <c r="K1572" t="inlineStr">
+        <is>
+          <t>0:23:47.807808</t>
+        </is>
+      </c>
+    </row>
+    <row r="1573">
+      <c r="A1573" t="inlineStr">
+        <is>
+          <t>2020-11-23 025725466784</t>
+        </is>
+      </c>
+      <c r="B1573" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1573" t="inlineStr">
+        <is>
+          <t>03:12:57.366755</t>
+        </is>
+      </c>
+      <c r="D1573" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1573" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1573" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1573" t="n">
+        <v>34800000</v>
+      </c>
+      <c r="H1573" t="n">
+        <v>150000</v>
+      </c>
+      <c r="I1573" s="5" t="n">
+        <v>44158.12321142111</v>
+      </c>
+      <c r="J1573" s="5" t="n">
+        <v>44158.13399730013</v>
+      </c>
+      <c r="K1573" t="inlineStr">
+        <is>
+          <t>0:15:31.899946</t>
+        </is>
+      </c>
+    </row>
+    <row r="1574">
+      <c r="A1574" t="inlineStr">
+        <is>
+          <t>2020-11-23 031301546716</t>
+        </is>
+      </c>
+      <c r="B1574" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1574" t="inlineStr">
+        <is>
+          <t>03:44:47.308645</t>
+        </is>
+      </c>
+      <c r="D1574" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1574" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1574" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1574" t="n">
+        <v>46400000</v>
+      </c>
+      <c r="H1574" t="n">
+        <v>200000</v>
+      </c>
+      <c r="I1574" s="5" t="n">
+        <v>44158.13404567958</v>
+      </c>
+      <c r="J1574" s="5" t="n">
+        <v>44158.15610310903</v>
+      </c>
+      <c r="K1574" t="inlineStr">
+        <is>
+          <t>0:31:45.761904</t>
+        </is>
+      </c>
+    </row>
+    <row r="1575">
+      <c r="A1575" t="inlineStr">
+        <is>
+          <t>2020-11-23 034449017175</t>
+        </is>
+      </c>
+      <c r="B1575" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1575" t="inlineStr">
+        <is>
+          <t>04:05:28.501660</t>
+        </is>
+      </c>
+      <c r="D1575" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1575" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1575" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1575" t="n">
+        <v>46400000</v>
+      </c>
+      <c r="H1575" t="n">
+        <v>200000</v>
+      </c>
+      <c r="I1575" s="5" t="n">
+        <v>44158.15612288397</v>
+      </c>
+      <c r="J1575" s="5" t="n">
+        <v>44158.17046876884</v>
+      </c>
+      <c r="K1575" t="inlineStr">
+        <is>
+          <t>0:20:39.484453</t>
+        </is>
+      </c>
+    </row>
+    <row r="1576">
+      <c r="A1576" t="inlineStr">
+        <is>
+          <t>2020-11-23 040532763931</t>
+        </is>
+      </c>
+      <c r="B1576" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1576" t="inlineStr">
+        <is>
+          <t>04:45:14.279737</t>
+        </is>
+      </c>
+      <c r="D1576" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1576" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1576" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1576" t="n">
+        <v>58000000</v>
+      </c>
+      <c r="H1576" t="n">
+        <v>250000</v>
+      </c>
+      <c r="I1576" s="5" t="n">
+        <v>44158.17051810105</v>
+      </c>
+      <c r="J1576" s="5" t="n">
+        <v>44158.1980819411</v>
+      </c>
+      <c r="K1576" t="inlineStr">
+        <is>
+          <t>0:39:41.515780</t>
+        </is>
+      </c>
+    </row>
+    <row r="1577">
+      <c r="A1577" t="inlineStr">
+        <is>
+          <t>2020-11-23 044516003580</t>
+        </is>
+      </c>
+      <c r="B1577" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1577" t="inlineStr">
+        <is>
+          <t>05:11:12.302686</t>
+        </is>
+      </c>
+      <c r="D1577" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1577" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1577" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1577" t="n">
+        <v>58000000</v>
+      </c>
+      <c r="H1577" t="n">
+        <v>250000</v>
+      </c>
+      <c r="I1577" s="5" t="n">
+        <v>44158.1981018933</v>
+      </c>
+      <c r="J1577" s="5" t="n">
+        <v>44158.21611461413</v>
+      </c>
+      <c r="K1577" t="inlineStr">
+        <is>
+          <t>0:25:56.299082</t>
+        </is>
+      </c>
+    </row>
+    <row r="1578">
+      <c r="A1578" t="inlineStr">
+        <is>
+          <t>2020-11-23 051116913519</t>
+        </is>
+      </c>
+      <c r="B1578" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1578" t="inlineStr">
+        <is>
+          <t>05:58:56.381906</t>
+        </is>
+      </c>
+      <c r="D1578" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1578" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1578" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1578" t="n">
+        <v>69600000</v>
+      </c>
+      <c r="H1578" t="n">
+        <v>300000</v>
+      </c>
+      <c r="I1578" s="5" t="n">
+        <v>44158.21616798054</v>
+      </c>
+      <c r="J1578" s="5" t="n">
+        <v>44158.24926367913</v>
+      </c>
+      <c r="K1578" t="inlineStr">
+        <is>
+          <t>0:47:39.468358</t>
+        </is>
+      </c>
+    </row>
+    <row r="1579">
+      <c r="A1579" t="inlineStr">
+        <is>
+          <t>2020-11-23 055858090862</t>
+        </is>
+      </c>
+      <c r="B1579" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1579" t="inlineStr">
+        <is>
+          <t>06:30:03.519950</t>
+        </is>
+      </c>
+      <c r="D1579" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1579" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1579" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1579" t="n">
+        <v>69600000</v>
+      </c>
+      <c r="H1579" t="n">
+        <v>300000</v>
+      </c>
+      <c r="I1579" s="5" t="n">
+        <v>44158.24928345905</v>
+      </c>
+      <c r="J1579" s="5" t="n">
+        <v>44158.27087407318</v>
+      </c>
+      <c r="K1579" t="inlineStr">
+        <is>
+          <t>0:31:05.429061</t>
+        </is>
+      </c>
+    </row>
+    <row r="1580">
+      <c r="A1580" t="inlineStr">
+        <is>
+          <t>2020-11-23 063008071534</t>
+        </is>
+      </c>
+      <c r="B1580" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1580" t="inlineStr">
+        <is>
+          <t>07:26:08.637220</t>
+        </is>
+      </c>
+      <c r="D1580" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1580" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1580" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1580" t="n">
+        <v>81200000</v>
+      </c>
+      <c r="H1580" t="n">
+        <v>350000</v>
+      </c>
+      <c r="I1580" s="5" t="n">
+        <v>44158.27092675387</v>
+      </c>
+      <c r="J1580" s="5" t="n">
+        <v>44158.30982218972</v>
+      </c>
+      <c r="K1580" t="inlineStr">
+        <is>
+          <t>0:56:00.565658</t>
+        </is>
+      </c>
+    </row>
+    <row r="1581">
+      <c r="A1581" t="inlineStr">
+        <is>
+          <t>2020-11-23 072610336490</t>
+        </is>
+      </c>
+      <c r="B1581" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1581" t="inlineStr">
+        <is>
+          <t>08:01:55.240663</t>
+        </is>
+      </c>
+      <c r="D1581" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1581" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1581" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1581" t="n">
+        <v>81200000</v>
+      </c>
+      <c r="H1581" t="n">
+        <v>350000</v>
+      </c>
+      <c r="I1581" s="5" t="n">
+        <v>44158.30984185751</v>
+      </c>
+      <c r="J1581" s="5" t="n">
+        <v>44158.33466713699</v>
+      </c>
+      <c r="K1581" t="inlineStr">
+        <is>
+          <t>0:35:44.904146</t>
+        </is>
+      </c>
+    </row>
+    <row r="1582">
+      <c r="A1582" t="inlineStr">
+        <is>
+          <t>2020-11-23 080200217371</t>
+        </is>
+      </c>
+      <c r="B1582" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1582" t="inlineStr">
+        <is>
+          <t>09:05:14.739751</t>
+        </is>
+      </c>
+      <c r="D1582" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1582" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1582" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1582" t="n">
+        <v>92800000</v>
+      </c>
+      <c r="H1582" t="n">
+        <v>400000</v>
+      </c>
+      <c r="I1582" s="5" t="n">
+        <v>44158.33472473809</v>
+      </c>
+      <c r="J1582" s="5" t="n">
+        <v>44158.37864282087</v>
+      </c>
+      <c r="K1582" t="inlineStr">
+        <is>
+          <t>1:03:14.522351</t>
+        </is>
+      </c>
+    </row>
+    <row r="1583">
+      <c r="A1583" t="inlineStr">
+        <is>
+          <t>2020-11-23 090516472542</t>
+        </is>
+      </c>
+      <c r="B1583" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1583" t="inlineStr">
+        <is>
+          <t>09:46:13.162362</t>
+        </is>
+      </c>
+      <c r="D1583" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1583" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1583" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1583" t="n">
+        <v>92800000</v>
+      </c>
+      <c r="H1583" t="n">
+        <v>400000</v>
+      </c>
+      <c r="I1583" s="5" t="n">
+        <v>44158.37866287665</v>
+      </c>
+      <c r="J1583" s="5" t="n">
+        <v>44158.40709678533</v>
+      </c>
+      <c r="K1583" t="inlineStr">
+        <is>
+          <t>0:40:56.689710</t>
+        </is>
+      </c>
+    </row>
+    <row r="1584">
+      <c r="A1584" t="inlineStr">
+        <is>
+          <t>2020-11-23 094618166507</t>
+        </is>
+      </c>
+      <c r="B1584" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1584" t="inlineStr">
+        <is>
+          <t>10:57:08.031845</t>
+        </is>
+      </c>
+      <c r="D1584" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1584" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1584" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1584" t="n">
+        <v>104400000</v>
+      </c>
+      <c r="H1584" t="n">
+        <v>450000</v>
+      </c>
+      <c r="I1584" s="5" t="n">
+        <v>44158.40715470494</v>
+      </c>
+      <c r="J1584" s="5" t="n">
+        <v>44158.4563429608</v>
+      </c>
+      <c r="K1584" t="inlineStr">
+        <is>
+          <t>1:10:49.865306</t>
+        </is>
+      </c>
+    </row>
+    <row r="1585">
+      <c r="A1585" t="inlineStr">
+        <is>
+          <t>2020-11-23 105709743315</t>
+        </is>
+      </c>
+      <c r="B1585" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1585" t="inlineStr">
+        <is>
+          <t>11:43:08.277033</t>
+        </is>
+      </c>
+      <c r="D1585" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1585" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1585" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1585" t="n">
+        <v>104400000</v>
+      </c>
+      <c r="H1585" t="n">
+        <v>450000</v>
+      </c>
+      <c r="I1585" s="5" t="n">
+        <v>44158.45636276985</v>
+      </c>
+      <c r="J1585" s="5" t="n">
+        <v>44158.48829024296</v>
+      </c>
+      <c r="K1585" t="inlineStr">
+        <is>
+          <t>0:45:58.533677</t>
+        </is>
+      </c>
+    </row>
+    <row r="1586">
+      <c r="A1586" t="inlineStr">
+        <is>
+          <t>2020-11-23 114313737510</t>
+        </is>
+      </c>
+      <c r="B1586" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1586" t="inlineStr">
+        <is>
+          <t>13:02:28.191770</t>
+        </is>
+      </c>
+      <c r="D1586" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1586" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1586" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1586" t="n">
+        <v>116000000</v>
+      </c>
+      <c r="H1586" t="n">
+        <v>500000</v>
+      </c>
+      <c r="I1586" s="5" t="n">
+        <v>44158.4883534434</v>
+      </c>
+      <c r="J1586" s="5" t="n">
+        <v>44158.54338184889</v>
+      </c>
+      <c r="K1586" t="inlineStr">
+        <is>
+          <t>1:19:14.454234</t>
+        </is>
+      </c>
+    </row>
+    <row r="1587">
+      <c r="A1587" t="inlineStr">
+        <is>
+          <t>2020-11-23 130229912887</t>
+        </is>
+      </c>
+      <c r="B1587" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1587" t="inlineStr">
+        <is>
+          <t>13:54:15.900339</t>
+        </is>
+      </c>
+      <c r="D1587" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1587" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1587" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1587" t="n">
+        <v>116000000</v>
+      </c>
+      <c r="H1587" t="n">
+        <v>500000</v>
+      </c>
+      <c r="I1587" s="5" t="n">
+        <v>44158.54340176952</v>
+      </c>
+      <c r="J1587" s="5" t="n">
+        <v>44158.57935069807</v>
+      </c>
+      <c r="K1587" t="inlineStr">
+        <is>
+          <t>0:51:45.987425</t>
+        </is>
+      </c>
+    </row>
+    <row r="1588">
+      <c r="A1588" t="inlineStr">
+        <is>
+          <t>2020-11-23 135421383735</t>
+        </is>
+      </c>
+      <c r="B1588" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1588" t="inlineStr">
+        <is>
+          <t>15:22:14.789052</t>
+        </is>
+      </c>
+      <c r="D1588" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1588" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1588" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1588" t="n">
+        <v>127600000</v>
+      </c>
+      <c r="H1588" t="n">
+        <v>550000</v>
+      </c>
+      <c r="I1588" s="5" t="n">
+        <v>44158.5794141636</v>
+      </c>
+      <c r="J1588" s="5" t="n">
+        <v>44158.64044894705</v>
+      </c>
+      <c r="K1588" t="inlineStr">
+        <is>
+          <t>1:27:53.405290</t>
+        </is>
+      </c>
+    </row>
+    <row r="1589">
+      <c r="A1589" t="inlineStr">
+        <is>
+          <t>2020-11-23 152216551278</t>
+        </is>
+      </c>
+      <c r="B1589" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1589" t="inlineStr">
+        <is>
+          <t>16:19:26.997190</t>
+        </is>
+      </c>
+      <c r="D1589" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1589" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1589" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1589" t="n">
+        <v>127600000</v>
+      </c>
+      <c r="H1589" t="n">
+        <v>550000</v>
+      </c>
+      <c r="I1589" s="5" t="n">
+        <v>44158.6404693435</v>
+      </c>
+      <c r="J1589" s="5" t="n">
+        <v>44158.68017357827</v>
+      </c>
+      <c r="K1589" t="inlineStr">
+        <is>
+          <t>0:57:10.445885</t>
+        </is>
+      </c>
+    </row>
+    <row r="1590">
+      <c r="A1590" t="inlineStr">
+        <is>
+          <t>2020-11-23 161932729252</t>
+        </is>
+      </c>
+      <c r="B1590" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1590" t="inlineStr">
+        <is>
+          <t>17:55:33.752517</t>
+        </is>
+      </c>
+      <c r="D1590" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1590" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1590" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1590" t="n">
+        <v>139200000</v>
+      </c>
+      <c r="H1590" t="n">
+        <v>600000</v>
+      </c>
+      <c r="I1590" s="5" t="n">
+        <v>44158.6802399219</v>
+      </c>
+      <c r="J1590" s="5" t="n">
+        <v>44158.74691843156</v>
+      </c>
+      <c r="K1590" t="inlineStr">
+        <is>
+          <t>1:36:01.023235</t>
+        </is>
+      </c>
+    </row>
+    <row r="1591">
+      <c r="A1591" t="inlineStr">
+        <is>
+          <t>2020-11-23 175535553798</t>
+        </is>
+      </c>
+      <c r="B1591" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1591" t="inlineStr">
+        <is>
+          <t>18:57:56.610849</t>
+        </is>
+      </c>
+      <c r="D1591" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1591" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1591" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1591" t="n">
+        <v>139200000</v>
+      </c>
+      <c r="H1591" t="n">
+        <v>600000</v>
+      </c>
+      <c r="I1591" s="5" t="n">
+        <v>44158.74693928007</v>
+      </c>
+      <c r="J1591" s="5" t="n">
+        <v>44158.79023855119</v>
+      </c>
+      <c r="K1591" t="inlineStr">
+        <is>
+          <t>1:02:21.057025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1592">
+      <c r="A1592" t="inlineStr">
+        <is>
+          <t>2020-11-23 185802630772</t>
+        </is>
+      </c>
+      <c r="B1592" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1592" t="inlineStr">
+        <is>
+          <t>20:41:58.808763</t>
+        </is>
+      </c>
+      <c r="D1592" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1592" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1592" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1592" t="n">
+        <v>150800000</v>
+      </c>
+      <c r="H1592" t="n">
+        <v>650000</v>
+      </c>
+      <c r="I1592" s="5" t="n">
+        <v>44158.79030822653</v>
+      </c>
+      <c r="J1592" s="5" t="n">
+        <v>44158.86248621221</v>
+      </c>
+      <c r="K1592" t="inlineStr">
+        <is>
+          <t>1:43:56.177963</t>
+        </is>
+      </c>
+    </row>
+    <row r="1593">
+      <c r="A1593" t="inlineStr">
+        <is>
+          <t>2020-11-23 204200549877</t>
+        </is>
+      </c>
+      <c r="B1593" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1593" t="inlineStr">
+        <is>
+          <t>21:49:20.335037</t>
+        </is>
+      </c>
+      <c r="D1593" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1593" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1593" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1593" t="n">
+        <v>150800000</v>
+      </c>
+      <c r="H1593" t="n">
+        <v>650000</v>
+      </c>
+      <c r="I1593" s="5" t="n">
+        <v>44158.86250636432</v>
+      </c>
+      <c r="J1593" s="5" t="n">
+        <v>44158.90926313669</v>
+      </c>
+      <c r="K1593" t="inlineStr">
+        <is>
+          <t>1:07:19.785133</t>
+        </is>
+      </c>
+    </row>
+    <row r="1594">
+      <c r="A1594" t="inlineStr">
+        <is>
+          <t>2020-11-23 214926845392</t>
+        </is>
+      </c>
+      <c r="B1594" s="4" t="n">
+        <v>44158</v>
+      </c>
+      <c r="C1594" t="inlineStr">
+        <is>
+          <t>23:42:22.116167</t>
+        </is>
+      </c>
+      <c r="D1594" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1594" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1594" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1594" t="n">
+        <v>162400000</v>
+      </c>
+      <c r="H1594" t="n">
+        <v>700000</v>
+      </c>
+      <c r="I1594" s="5" t="n">
+        <v>44158.90933848833</v>
+      </c>
+      <c r="J1594" s="5" t="n">
+        <v>44158.98775597385</v>
+      </c>
+      <c r="K1594" t="inlineStr">
+        <is>
+          <t>1:52:55.270748</t>
+        </is>
+      </c>
+    </row>
+    <row r="1595">
+      <c r="A1595" t="inlineStr">
+        <is>
+          <t>2020-11-23 234223884594</t>
+        </is>
+      </c>
+      <c r="B1595" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1595" t="inlineStr">
+        <is>
+          <t>00:54:53.403299</t>
+        </is>
+      </c>
+      <c r="D1595" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1595" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1595" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1595" t="n">
+        <v>162400000</v>
+      </c>
+      <c r="H1595" t="n">
+        <v>700000</v>
+      </c>
+      <c r="I1595" s="5" t="n">
+        <v>44158.98777644206</v>
+      </c>
+      <c r="J1595" s="5" t="n">
+        <v>44159.03811809341</v>
+      </c>
+      <c r="K1595" t="inlineStr">
+        <is>
+          <t>1:12:29.518677</t>
+        </is>
+      </c>
+    </row>
+    <row r="1596">
+      <c r="A1596" t="inlineStr">
+        <is>
+          <t>2020-11-24 005500192348</t>
+        </is>
+      </c>
+      <c r="B1596" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1596" t="inlineStr">
+        <is>
+          <t>02:55:01.369610</t>
+        </is>
+      </c>
+      <c r="D1596" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1596" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1596" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1596" t="n">
+        <v>174000000</v>
+      </c>
+      <c r="H1596" t="n">
+        <v>750000</v>
+      </c>
+      <c r="I1596" s="5" t="n">
+        <v>44159.03819667069</v>
+      </c>
+      <c r="J1596" s="5" t="n">
+        <v>44159.12154362941</v>
+      </c>
+      <c r="K1596" t="inlineStr">
+        <is>
+          <t>2:00:01.177233</t>
+        </is>
+      </c>
+    </row>
+    <row r="1597">
+      <c r="A1597" t="inlineStr">
+        <is>
+          <t>2020-11-24 025503173321</t>
+        </is>
+      </c>
+      <c r="B1597" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1597" t="inlineStr">
+        <is>
+          <t>04:12:58.599734</t>
+        </is>
+      </c>
+      <c r="D1597" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1597" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1597" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1597" t="n">
+        <v>174000000</v>
+      </c>
+      <c r="H1597" t="n">
+        <v>750000</v>
+      </c>
+      <c r="I1597" s="5" t="n">
+        <v>44159.12156450603</v>
+      </c>
+      <c r="J1597" s="5" t="n">
+        <v>44159.17567823734</v>
+      </c>
+      <c r="K1597" t="inlineStr">
+        <is>
+          <t>1:17:55.426385</t>
+        </is>
+      </c>
+    </row>
+    <row r="1598">
+      <c r="A1598" t="inlineStr">
+        <is>
+          <t>2020-11-24 041305981224</t>
+        </is>
+      </c>
+      <c r="B1598" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1598" t="inlineStr">
+        <is>
+          <t>06:21:09.893800</t>
+        </is>
+      </c>
+      <c r="D1598" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1598" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1598" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1598" t="n">
+        <v>185600000</v>
+      </c>
+      <c r="H1598" t="n">
+        <v>800000</v>
+      </c>
+      <c r="I1598" s="5" t="n">
+        <v>44159.17576367158</v>
+      </c>
+      <c r="J1598" s="5" t="n">
+        <v>44159.26469784457</v>
+      </c>
+      <c r="K1598" t="inlineStr">
+        <is>
+          <t>2:08:03.912548</t>
+        </is>
+      </c>
+    </row>
+    <row r="1599">
+      <c r="A1599" t="inlineStr">
+        <is>
+          <t>2020-11-24 062111640794</t>
+        </is>
+      </c>
+      <c r="B1599" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1599" t="inlineStr">
+        <is>
+          <t>07:44:12.101179</t>
+        </is>
+      </c>
+      <c r="D1599" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1599" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1599" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1599" t="n">
+        <v>185600000</v>
+      </c>
+      <c r="H1599" t="n">
+        <v>800000</v>
+      </c>
+      <c r="I1599" s="5" t="n">
+        <v>44159.26471806475</v>
+      </c>
+      <c r="J1599" s="5" t="n">
+        <v>44159.32236228186</v>
+      </c>
+      <c r="K1599" t="inlineStr">
+        <is>
+          <t>1:23:00.460358</t>
+        </is>
+      </c>
+    </row>
+    <row r="1600">
+      <c r="A1600" t="inlineStr">
+        <is>
+          <t>2020-11-24 074420112165</t>
+        </is>
+      </c>
+      <c r="B1600" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1600" t="inlineStr">
+        <is>
+          <t>09:59:38.585042</t>
+        </is>
+      </c>
+      <c r="D1600" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1600" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1600" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1600" t="n">
+        <v>197200000</v>
+      </c>
+      <c r="H1600" t="n">
+        <v>850000</v>
+      </c>
+      <c r="I1600" s="5" t="n">
+        <v>44159.32245500191</v>
+      </c>
+      <c r="J1600" s="5" t="n">
+        <v>44159.41641880801</v>
+      </c>
+      <c r="K1600" t="inlineStr">
+        <is>
+          <t>2:15:18.472847</t>
+        </is>
+      </c>
+    </row>
+    <row r="1601">
+      <c r="A1601" t="inlineStr">
+        <is>
+          <t>2020-11-24 095940342694</t>
+        </is>
+      </c>
+      <c r="B1601" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1601" t="inlineStr">
+        <is>
+          <t>11:26:24.617072</t>
+        </is>
+      </c>
+      <c r="D1601" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1601" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1601" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1601" t="n">
+        <v>197200000</v>
+      </c>
+      <c r="H1601" t="n">
+        <v>850000</v>
+      </c>
+      <c r="I1601" s="5" t="n">
+        <v>44159.41643915155</v>
+      </c>
+      <c r="J1601" s="5" t="n">
+        <v>44159.47667380832</v>
+      </c>
+      <c r="K1601" t="inlineStr">
+        <is>
+          <t>1:26:44.274346</t>
+        </is>
+      </c>
+    </row>
+    <row r="1602">
+      <c r="A1602" t="inlineStr">
+        <is>
+          <t>2020-11-24 112632059581</t>
+        </is>
+      </c>
+      <c r="B1602" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1602" t="inlineStr">
+        <is>
+          <t>13:50:47.465638</t>
+        </is>
+      </c>
+      <c r="D1602" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1602" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1602" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1602" t="n">
+        <v>208800000</v>
+      </c>
+      <c r="H1602" t="n">
+        <v>900000</v>
+      </c>
+      <c r="I1602" s="5" t="n">
+        <v>44159.47675994886</v>
+      </c>
+      <c r="J1602" s="5" t="n">
+        <v>44159.57693825934</v>
+      </c>
+      <c r="K1602" t="inlineStr">
+        <is>
+          <t>2:24:15.406026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1603">
+      <c r="A1603" t="inlineStr">
+        <is>
+          <t>2020-11-24 135049281694</t>
+        </is>
+      </c>
+      <c r="B1603" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1603" t="inlineStr">
+        <is>
+          <t>15:24:22.195287</t>
+        </is>
+      </c>
+      <c r="D1603" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1603" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1603" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1603" t="n">
+        <v>208800000</v>
+      </c>
+      <c r="H1603" t="n">
+        <v>900000</v>
+      </c>
+      <c r="I1603" s="5" t="n">
+        <v>44159.57695927886</v>
+      </c>
+      <c r="J1603" s="5" t="n">
+        <v>44159.64192355624</v>
+      </c>
+      <c r="K1603" t="inlineStr">
+        <is>
+          <t>1:33:32.913565</t>
+        </is>
+      </c>
+    </row>
+    <row r="1604">
+      <c r="A1604" t="inlineStr">
+        <is>
+          <t>2020-11-24 152430477949</t>
+        </is>
+      </c>
+      <c r="B1604" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1604" t="inlineStr">
+        <is>
+          <t>17:57:04.172048</t>
+        </is>
+      </c>
+      <c r="D1604" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1604" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1604" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1604" t="n">
+        <v>220400000</v>
+      </c>
+      <c r="H1604" t="n">
+        <v>950000</v>
+      </c>
+      <c r="I1604" s="5" t="n">
+        <v>44159.64201942071</v>
+      </c>
+      <c r="J1604" s="5" t="n">
+        <v>44159.74796495394</v>
+      </c>
+      <c r="K1604" t="inlineStr">
+        <is>
+          <t>2:32:33.694071</t>
+        </is>
+      </c>
+    </row>
+    <row r="1605">
+      <c r="A1605" t="inlineStr">
+        <is>
+          <t>2020-11-24 175705966082</t>
+        </is>
+      </c>
+      <c r="B1605" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1605" t="inlineStr">
+        <is>
+          <t>19:35:43.410513</t>
+        </is>
+      </c>
+      <c r="D1605" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1605" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1605" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1605" t="n">
+        <v>220400000</v>
+      </c>
+      <c r="H1605" t="n">
+        <v>950000</v>
+      </c>
+      <c r="I1605" s="5" t="n">
+        <v>44159.74798571854</v>
+      </c>
+      <c r="J1605" s="5" t="n">
+        <v>44159.81647465812</v>
+      </c>
+      <c r="K1605" t="inlineStr">
+        <is>
+          <t>1:38:37.444380</t>
+        </is>
+      </c>
+    </row>
+    <row r="1606">
+      <c r="A1606" t="inlineStr">
+        <is>
+          <t>2020-11-24 193551268309</t>
+        </is>
+      </c>
+      <c r="B1606" s="4" t="n">
+        <v>44159</v>
+      </c>
+      <c r="C1606" t="inlineStr">
+        <is>
+          <t>22:16:19.031193</t>
+        </is>
+      </c>
+      <c r="D1606" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="E1606" t="inlineStr">
+        <is>
+          <t>single client / single write</t>
+        </is>
+      </c>
+      <c r="F1606" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1606" t="n">
+        <v>232000000</v>
+      </c>
+      <c r="H1606" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="I1606" s="5" t="n">
+        <v>44159.81656560543</v>
+      </c>
+      <c r="J1606" s="5" t="n">
+        <v>44159.92799804594</v>
+      </c>
+      <c r="K1606" t="inlineStr">
+        <is>
+          <t>2:40:27.762860</t>
+        </is>
+      </c>
+    </row>
+    <row r="1607">
+      <c r="A1607" t="inlineStr">
+        <is>
+          <t>2020-11-24 221620794070</t>
+        </is>
+      </c>
+      <c r="B1607" s="4" t="n">
+        <v>44160</v>
+      </c>
+      <c r="C1607" t="inlineStr">
+        <is>
+          <t>00:00:23.226276</t>
+        </is>
+      </c>
+      <c r="D1607" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E1607" t="inlineStr">
+        <is>
+          <t>single cliente / single read</t>
+        </is>
+      </c>
+      <c r="F1607" t="inlineStr">
+        <is>
+          <t>/samples</t>
+        </is>
+      </c>
+      <c r="G1607" t="n">
+        <v>232000000</v>
+      </c>
+      <c r="H1607" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="I1607" s="5" t="n">
+        <v>44159.92801844989</v>
+      </c>
+      <c r="J1607" s="5" t="n">
+        <v>44160.00026882232</v>
+      </c>
+      <c r="K1607" t="inlineStr">
+        <is>
+          <t>1:44:02.432179</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>